<commit_message>
update umay substrate grwoth
</commit_message>
<xml_diff>
--- a/data/Biolog Daten PM2A Platten.xlsx
+++ b/data/Biolog Daten PM2A Platten.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bio4-fs\data\iAMBAll\Lena Ullmann\BIOLOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Desktop\Forschungspraktikum\Ustilago_maydis-GEM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C9439-9C5C-4224-A576-F5BB3B8A9DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="12075"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -278,7 +279,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -294,7 +295,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -369,6 +370,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -404,6 +422,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -579,20 +614,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -600,7 +635,7 @@
         <v>44335</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -611,7 +646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -622,7 +657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -633,7 +668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -644,16 +679,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:M30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="B2" s="2">
         <v>1</v>
@@ -692,7 +727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -733,7 +768,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -774,7 +809,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -815,7 +850,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -856,7 +891,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -897,7 +932,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,7 +973,7 @@
         <v>0.14799999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -979,7 +1014,7 @@
         <v>0.14599999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1020,7 +1055,7 @@
         <v>0.186</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
       <c r="B12" s="2">
         <v>1</v>
@@ -1059,7 +1094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1135,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1141,7 +1176,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1217,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1223,7 +1258,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1299,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1340,7 @@
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +1381,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1422,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="17"/>
       <c r="B22" s="2">
         <v>1</v>
@@ -1426,7 +1461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1502,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
@@ -1508,7 +1543,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1549,7 +1584,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1625,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -1631,7 +1666,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1672,7 +1707,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1713,7 +1748,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1760,16 +1795,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <v>1</v>
@@ -1808,7 +1843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1884,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1890,7 +1925,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1931,7 +1966,7 @@
         <v>1.0469999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +2007,7 @@
         <v>1.194</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2013,7 +2048,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2054,7 +2089,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2130,7 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2136,7 +2171,7 @@
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="2">
         <v>1</v>
@@ -2175,7 +2210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2251,7 @@
         <v>0.107</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2257,7 +2292,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2333,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
@@ -2339,7 +2374,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
@@ -2380,7 +2415,7 @@
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -2421,7 +2456,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -2462,7 +2497,7 @@
         <v>0.217</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2503,7 +2538,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="2">
         <v>1</v>
@@ -2542,7 +2577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2618,7 @@
         <v>0.377</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
@@ -2624,7 +2659,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
@@ -2665,7 +2700,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
@@ -2706,7 +2741,7 @@
         <v>1.0569999999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
@@ -2747,7 +2782,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -2788,7 +2823,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -2829,7 +2864,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -2876,16 +2911,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="B2" s="2">
         <v>1</v>
@@ -2924,7 +2959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +3000,7 @@
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3006,7 +3041,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3047,7 +3082,7 @@
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3088,7 +3123,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -3129,7 +3164,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3170,7 +3205,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -3211,7 +3246,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3252,370 +3287,370 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="17"/>
+      <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C22" s="2">
         <v>2</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D22" s="2">
         <v>3</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E22" s="2">
         <v>4</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F22" s="2">
         <v>5</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G22" s="2">
         <v>6</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H22" s="2">
         <v>7</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I22" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J22" s="2">
         <v>9</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K22" s="2">
         <v>10</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L22" s="2">
         <v>11</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M22" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="4">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D23" s="4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F23" s="4">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="H23" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J23" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K23" s="6">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="M23" s="4">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D24" s="4">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="G24" s="10">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="H24" s="14">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.187</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.187</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="M24" s="4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.214</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1.198</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0.752</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="I25" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.127</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0.224</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="M25" s="16">
+        <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.873</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.252</v>
+      </c>
+      <c r="E26" s="4">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="J26" s="4">
+        <v>9.4E-2</v>
+      </c>
+      <c r="K26" s="16">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="M26" s="7">
+        <v>1.0589999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0.33</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.182</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="L27" s="12">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E28" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.157</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0.996</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0.23599999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="4">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="C29" s="4">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="D29" s="4">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="E29" s="4">
-        <v>7.8E-2</v>
-      </c>
-      <c r="F29" s="4">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0.23</v>
+        <v>6</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="G29" s="4">
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H29" s="4">
-        <v>9.8000000000000004E-2</v>
+        <v>0.04</v>
       </c>
       <c r="I29" s="4">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="J29" s="4">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="K29" s="6">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="L29" s="3">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="M29" s="4">
-        <v>8.5000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="L29" s="15">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="D30" s="4">
-        <v>8.5000000000000006E-2</v>
+        <v>7</v>
+      </c>
+      <c r="B30" s="16">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.189</v>
       </c>
       <c r="E30" s="5">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="F30" s="14">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1.3140000000000001</v>
-      </c>
-      <c r="H30" s="14">
-        <v>0.77100000000000002</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0.187</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0.187</v>
-      </c>
-      <c r="K30" s="6">
-        <v>0.67300000000000004</v>
-      </c>
-      <c r="L30" s="8">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="M30" s="4">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G30" s="4">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0.214</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1.198</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="G31" s="16">
-        <v>0.752</v>
-      </c>
-      <c r="H31" s="3">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="I31" s="4">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.127</v>
-      </c>
-      <c r="K31" s="5">
-        <v>0.224</v>
-      </c>
-      <c r="L31" s="12">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="M31" s="16">
-        <v>0.72199999999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0.873</v>
-      </c>
-      <c r="C32" s="11">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0.252</v>
-      </c>
-      <c r="E32" s="4">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="F32" s="12">
-        <v>0.41199999999999998</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="H32" s="8">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="I32" s="14">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="J32" s="4">
-        <v>9.4E-2</v>
-      </c>
-      <c r="K32" s="16">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="L32" s="13">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="M32" s="7">
-        <v>1.0589999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="4">
+      <c r="H30" s="4">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="C33" s="4">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="D33" s="13">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="E33" s="5">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="F33" s="4">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="G33" s="16">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="H33" s="13">
-        <v>0.33</v>
-      </c>
-      <c r="I33" s="8">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="J33" s="3">
-        <v>0.182</v>
-      </c>
-      <c r="K33" s="5">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="L33" s="12">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="M33" s="3">
-        <v>0.17399999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="8">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="C34" s="12">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="D34" s="12">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="E34" s="4">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.157</v>
-      </c>
-      <c r="G34" s="10">
-        <v>1.2669999999999999</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="I34" s="11">
-        <v>0.996</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="K34" s="15">
-        <v>0.54</v>
-      </c>
-      <c r="L34" s="3">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="M34" s="5">
-        <v>0.23599999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="5">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="C35" s="6">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="F35" s="12">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="G35" s="4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="H35" s="4">
+      <c r="I30" s="4">
         <v>0.04</v>
       </c>
-      <c r="I35" s="4">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="J35" s="8">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="K35" s="7">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="L35" s="15">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="M35" s="5">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="16">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="C36" s="12">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.189</v>
-      </c>
-      <c r="E36" s="5">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="F36" s="4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="G36" s="4">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="H36" s="4">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="I36" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="J36" s="15">
+      <c r="J30" s="15">
         <v>0.51700000000000002</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K30" s="3">
         <v>0.185</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L30" s="4">
         <v>0.122</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M30" s="3">
         <v>0.17399999999999999</v>
       </c>
     </row>

</xml_diff>